<commit_message>
Replaced "Finalization" and "Organization" by "Finalisation" and "Orgaaisation", respectively. Bolded "email"
</commit_message>
<xml_diff>
--- a/forms/Form-1DI_interim.xlsx
+++ b/forms/Form-1DI_interim.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-workflow\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420533EE-CE41-414E-9B95-9EAEF19653DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8DBF7A-2EC6-4CA6-8A02-0175CEC3D394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -48,12 +48,6 @@
     <t>Full name</t>
   </si>
   <si>
-    <t>e-mail</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
     <t>General information</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
   </si>
   <si>
     <t>Submission information</t>
-  </si>
-  <si>
-    <t>Finalization date</t>
   </si>
   <si>
     <t>Submission date</t>
@@ -170,6 +161,15 @@
   </si>
   <si>
     <t>1.0.0-interim</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Finalisation date</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1477,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="84" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="85"/>
       <c r="D2" s="85"/>
@@ -1514,17 +1514,17 @@
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1540,7 +1540,7 @@
     <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="9"/>
       <c r="C6" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1565,7 +1565,7 @@
       <c r="D8" s="83"/>
       <c r="E8" s="10"/>
       <c r="F8" s="83" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="G8" s="83"/>
       <c r="H8" s="11"/>
@@ -1586,12 +1586,12 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="14" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
-        <v>3</v>
+      <c r="F10" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="11"/>
@@ -1608,7 +1608,7 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="14" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="10"/>
@@ -1619,7 +1619,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="10"/>
@@ -1648,7 +1648,7 @@
     <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1668,7 +1668,7 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="10"/>
@@ -1679,7 +1679,7 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="53" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="10"/>
@@ -1690,7 +1690,7 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="52" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="10"/>
@@ -1719,7 +1719,7 @@
     <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="10"/>
@@ -1759,7 +1759,7 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9e764YFvhuYflrxNR7EzcULwaYOP9egrLMIFFxgVT80Ix5nVKzyC71Q8mK9m4F5eb4YoUVrEwlywdTU/UkJ0uA==" saltValue="aSkxjMwP4SqQZevgiUxLJw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vkHR2TUcSJSTXpTCvLOEWWRkCuAPrMSUnePY1u9iVpuuqEBi8djcHnwvg2Gwb0CYMq0yj1ImkzH6u62X0rYtPw==" saltValue="xTOasHLEM2uXGK5KFn205w==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="2" spans="1:212" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="84" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="85"/>
       <c r="D2" s="85"/>
@@ -2042,7 +2042,7 @@
       <c r="K3" s="88"/>
       <c r="L3" s="112"/>
       <c r="M3" s="108" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N3" s="109"/>
       <c r="O3" s="109"/>
@@ -2246,23 +2246,23 @@
     </row>
     <row r="4" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="90" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="91"/>
       <c r="D4" s="91"/>
       <c r="E4" s="91"/>
       <c r="F4" s="92"/>
       <c r="G4" s="99" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H4" s="100"/>
       <c r="I4" s="101"/>
       <c r="J4" s="99" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K4" s="101"/>
       <c r="L4" s="63" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M4" s="26"/>
       <c r="N4" s="27"/>
@@ -2477,7 +2477,7 @@
       <c r="J5" s="102"/>
       <c r="K5" s="104"/>
       <c r="L5" s="51" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M5" s="26"/>
       <c r="N5" s="27"/>
@@ -2692,7 +2692,7 @@
       <c r="J6" s="105"/>
       <c r="K6" s="107"/>
       <c r="L6" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M6" s="26"/>
       <c r="N6" s="27"/>
@@ -2897,37 +2897,37 @@
     </row>
     <row r="7" spans="1:212" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="55" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" s="60" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H7" s="58" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7" s="59" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J7" s="61" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K7" s="62" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L7" s="64" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="30"/>

</xml_diff>

<commit_message>
Fucking bolded text for "email"
</commit_message>
<xml_diff>
--- a/forms/Form-1DI_interim.xlsx
+++ b/forms/Form-1DI_interim.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-workflow\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8DBF7A-2EC6-4CA6-8A02-0175CEC3D394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2EF6D7-4964-4EF6-A494-6A693056FF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -795,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1144,6 +1144,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1590,7 +1591,7 @@
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="113" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="24"/>
@@ -1759,7 +1760,7 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vkHR2TUcSJSTXpTCvLOEWWRkCuAPrMSUnePY1u9iVpuuqEBi8djcHnwvg2Gwb0CYMq0yj1ImkzH6u62X0rYtPw==" saltValue="xTOasHLEM2uXGK5KFn205w==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/7xVg0ceMuuzokJMThBrAdiopJIb6BHbkZIVgGq2v7uaObo34M6L9tEZr4f1Z2V9Vs9cawMlPOx5010D36SdxA==" saltValue="dm+4gVFhSrhFRGTTKqMOHA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>

</xml_diff>

<commit_message>
Minor changes to forms.
</commit_message>
<xml_diff>
--- a/forms/Form-1DI_interim.xlsx
+++ b/forms/Form-1DI_interim.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-workflow\workflow\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2EF6D7-4964-4EF6-A494-6A693056FF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5308F77A-E9E5-49D7-B166-EECD4C2AE6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -795,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1144,7 +1144,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1478,7 +1477,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1590,7 @@
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="113" t="s">
+      <c r="F10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="24"/>

</xml_diff>